<commit_message>
10/01/24 commit - upated closest to pin hole # week 22
</commit_message>
<xml_diff>
--- a/public/results/Bottoms Up 2024 League Stats - Week 22.xlsx
+++ b/public/results/Bottoms Up 2024 League Stats - Week 22.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\CODE\golf-league-site\public\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\source\repos\golf-league-site\public\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E211127A-D0BE-4413-AA19-C79B0CD6B97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEB79EC-5047-4EC5-A632-E542B22DD17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="570" windowWidth="22305" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="1290" windowWidth="21945" windowHeight="14910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="14" r:id="rId1"/>
@@ -1458,7 +1458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1896,7 +1896,19 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1905,15 +1917,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1926,6 +1929,63 @@
     </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="19" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1972,54 +2032,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2032,35 +2044,12 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FEB32575-F33B-455F-81F3-7FDBFE07DE6C}"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF1A983"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2548,23 +2537,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -2578,23 +2567,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -3452,23 +3441,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -3482,23 +3471,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -4507,23 +4496,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -4537,23 +4526,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -5559,23 +5548,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -5589,23 +5578,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -6996,23 +6985,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -7026,23 +7015,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -8048,23 +8037,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -8078,23 +8067,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -8997,23 +8986,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -9027,23 +9016,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -10363,23 +10352,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -10393,23 +10382,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -11720,24 +11709,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="210" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="206"/>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
-      <c r="D2" s="206"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="206"/>
-      <c r="B3" s="206"/>
-      <c r="C3" s="206"/>
-      <c r="D3" s="206"/>
+      <c r="A3" s="210"/>
+      <c r="B3" s="210"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="210"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11774,23 +11763,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -11804,23 +11793,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -13131,24 +13120,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="210" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="206"/>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
-      <c r="D2" s="206"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="206"/>
-      <c r="B3" s="206"/>
-      <c r="C3" s="206"/>
-      <c r="D3" s="206"/>
+      <c r="A3" s="210"/>
+      <c r="B3" s="210"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="210"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13162,8 +13151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1EE897-404D-4ADC-856A-1E864FE4E3AA}">
   <dimension ref="A1:BH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX16" sqref="AX16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BJ15" sqref="BJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13211,252 +13200,252 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" s="1" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="175" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="199" t="s">
+      <c r="B1" s="176"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="184" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="168" t="s">
+      <c r="E1" s="169" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="169"/>
-      <c r="G1" s="168" t="s">
+      <c r="F1" s="170"/>
+      <c r="G1" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="169"/>
-      <c r="I1" s="168" t="s">
+      <c r="H1" s="170"/>
+      <c r="I1" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="169"/>
-      <c r="K1" s="168" t="s">
+      <c r="J1" s="170"/>
+      <c r="K1" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="169"/>
-      <c r="M1" s="168" t="s">
+      <c r="L1" s="170"/>
+      <c r="M1" s="169" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="169"/>
-      <c r="O1" s="168" t="s">
+      <c r="N1" s="170"/>
+      <c r="O1" s="169" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="168" t="s">
+      <c r="P1" s="170"/>
+      <c r="Q1" s="169" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="169"/>
-      <c r="S1" s="168" t="s">
+      <c r="R1" s="170"/>
+      <c r="S1" s="169" t="s">
         <v>90</v>
       </c>
-      <c r="T1" s="169"/>
-      <c r="U1" s="168" t="s">
+      <c r="T1" s="170"/>
+      <c r="U1" s="169" t="s">
         <v>93</v>
       </c>
-      <c r="V1" s="169"/>
-      <c r="W1" s="168" t="s">
+      <c r="V1" s="170"/>
+      <c r="W1" s="169" t="s">
         <v>95</v>
       </c>
-      <c r="X1" s="169"/>
-      <c r="Y1" s="168" t="s">
+      <c r="X1" s="170"/>
+      <c r="Y1" s="169" t="s">
         <v>96</v>
       </c>
-      <c r="Z1" s="169"/>
-      <c r="AA1" s="168" t="s">
+      <c r="Z1" s="170"/>
+      <c r="AA1" s="169" t="s">
         <v>105</v>
       </c>
-      <c r="AB1" s="169"/>
-      <c r="AC1" s="168" t="s">
+      <c r="AB1" s="170"/>
+      <c r="AC1" s="169" t="s">
         <v>110</v>
       </c>
-      <c r="AD1" s="169"/>
-      <c r="AE1" s="168" t="s">
+      <c r="AD1" s="170"/>
+      <c r="AE1" s="169" t="s">
         <v>112</v>
       </c>
-      <c r="AF1" s="169"/>
-      <c r="AG1" s="168" t="s">
+      <c r="AF1" s="170"/>
+      <c r="AG1" s="169" t="s">
         <v>113</v>
       </c>
-      <c r="AH1" s="169"/>
-      <c r="AI1" s="168" t="s">
+      <c r="AH1" s="170"/>
+      <c r="AI1" s="169" t="s">
         <v>115</v>
       </c>
-      <c r="AJ1" s="169"/>
-      <c r="AK1" s="168" t="s">
+      <c r="AJ1" s="170"/>
+      <c r="AK1" s="169" t="s">
         <v>116</v>
       </c>
-      <c r="AL1" s="169"/>
-      <c r="AM1" s="168" t="s">
+      <c r="AL1" s="170"/>
+      <c r="AM1" s="169" t="s">
         <v>118</v>
       </c>
-      <c r="AN1" s="169"/>
-      <c r="AO1" s="168" t="s">
+      <c r="AN1" s="170"/>
+      <c r="AO1" s="169" t="s">
         <v>119</v>
       </c>
-      <c r="AP1" s="169"/>
-      <c r="AQ1" s="168" t="s">
+      <c r="AP1" s="170"/>
+      <c r="AQ1" s="169" t="s">
         <v>120</v>
       </c>
-      <c r="AR1" s="169"/>
-      <c r="AS1" s="168" t="s">
+      <c r="AR1" s="170"/>
+      <c r="AS1" s="169" t="s">
         <v>124</v>
       </c>
-      <c r="AT1" s="169"/>
-      <c r="AU1" s="168" t="s">
+      <c r="AT1" s="170"/>
+      <c r="AU1" s="169" t="s">
         <v>125</v>
       </c>
-      <c r="AV1" s="169"/>
-      <c r="AW1" s="187" t="s">
+      <c r="AV1" s="170"/>
+      <c r="AW1" s="186" t="s">
         <v>35</v>
       </c>
-      <c r="AX1" s="175" t="s">
+      <c r="AX1" s="195" t="s">
         <v>111</v>
       </c>
       <c r="AY1" s="106"/>
-      <c r="AZ1" s="178" t="s">
+      <c r="AZ1" s="198" t="s">
         <v>103</v>
       </c>
-      <c r="BA1" s="179"/>
-      <c r="BB1" s="179"/>
-      <c r="BC1" s="180"/>
-      <c r="BD1" s="165" t="s">
+      <c r="BA1" s="199"/>
+      <c r="BB1" s="199"/>
+      <c r="BC1" s="200"/>
+      <c r="BD1" s="189" t="s">
         <v>109</v>
       </c>
-      <c r="BE1" s="172" t="s">
+      <c r="BE1" s="192" t="s">
         <v>104</v>
       </c>
-      <c r="BF1" s="173"/>
-      <c r="BG1" s="173"/>
-      <c r="BH1" s="174"/>
+      <c r="BF1" s="193"/>
+      <c r="BG1" s="193"/>
+      <c r="BH1" s="194"/>
     </row>
     <row r="2" spans="1:60" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="192"/>
-      <c r="B2" s="193"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="170">
+      <c r="A2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="171">
         <v>45418</v>
       </c>
-      <c r="F2" s="171"/>
-      <c r="G2" s="201">
+      <c r="F2" s="172"/>
+      <c r="G2" s="173">
         <v>45425</v>
       </c>
-      <c r="H2" s="202"/>
-      <c r="I2" s="201">
+      <c r="H2" s="174"/>
+      <c r="I2" s="173">
         <v>45432</v>
       </c>
-      <c r="J2" s="202"/>
-      <c r="K2" s="201">
+      <c r="J2" s="174"/>
+      <c r="K2" s="173">
         <v>45439</v>
       </c>
-      <c r="L2" s="202"/>
-      <c r="M2" s="201">
+      <c r="L2" s="174"/>
+      <c r="M2" s="173">
         <v>45446</v>
       </c>
-      <c r="N2" s="202"/>
-      <c r="O2" s="201">
+      <c r="N2" s="174"/>
+      <c r="O2" s="173">
         <v>45453</v>
       </c>
-      <c r="P2" s="202"/>
-      <c r="Q2" s="201">
+      <c r="P2" s="174"/>
+      <c r="Q2" s="173">
         <v>45460</v>
       </c>
-      <c r="R2" s="202"/>
-      <c r="S2" s="201">
+      <c r="R2" s="174"/>
+      <c r="S2" s="173">
         <v>45467</v>
       </c>
-      <c r="T2" s="202"/>
-      <c r="U2" s="201">
+      <c r="T2" s="174"/>
+      <c r="U2" s="173">
         <v>45474</v>
       </c>
-      <c r="V2" s="202"/>
-      <c r="W2" s="201">
+      <c r="V2" s="174"/>
+      <c r="W2" s="173">
         <v>45481</v>
       </c>
-      <c r="X2" s="202"/>
-      <c r="Y2" s="201">
+      <c r="X2" s="174"/>
+      <c r="Y2" s="173">
         <v>45488</v>
       </c>
-      <c r="Z2" s="202"/>
-      <c r="AA2" s="170">
+      <c r="Z2" s="174"/>
+      <c r="AA2" s="171">
         <v>45495</v>
       </c>
-      <c r="AB2" s="171"/>
-      <c r="AC2" s="170">
+      <c r="AB2" s="172"/>
+      <c r="AC2" s="171">
         <v>45502</v>
       </c>
-      <c r="AD2" s="171"/>
-      <c r="AE2" s="170">
+      <c r="AD2" s="172"/>
+      <c r="AE2" s="171">
         <v>45509</v>
       </c>
-      <c r="AF2" s="171"/>
-      <c r="AG2" s="170">
+      <c r="AF2" s="172"/>
+      <c r="AG2" s="171">
         <v>45516</v>
       </c>
-      <c r="AH2" s="171"/>
-      <c r="AI2" s="170">
+      <c r="AH2" s="172"/>
+      <c r="AI2" s="171">
         <v>45523</v>
       </c>
-      <c r="AJ2" s="171"/>
-      <c r="AK2" s="170">
+      <c r="AJ2" s="172"/>
+      <c r="AK2" s="171">
         <v>45530</v>
       </c>
-      <c r="AL2" s="171"/>
-      <c r="AM2" s="170">
+      <c r="AL2" s="172"/>
+      <c r="AM2" s="171">
         <v>45537</v>
       </c>
-      <c r="AN2" s="171"/>
-      <c r="AO2" s="170">
+      <c r="AN2" s="172"/>
+      <c r="AO2" s="171">
         <v>45544</v>
       </c>
-      <c r="AP2" s="171"/>
-      <c r="AQ2" s="170">
+      <c r="AP2" s="172"/>
+      <c r="AQ2" s="171">
         <v>45551</v>
       </c>
-      <c r="AR2" s="171"/>
-      <c r="AS2" s="170">
+      <c r="AR2" s="172"/>
+      <c r="AS2" s="171">
         <v>45558</v>
       </c>
-      <c r="AT2" s="171"/>
-      <c r="AU2" s="170">
+      <c r="AT2" s="172"/>
+      <c r="AU2" s="171">
         <v>45565</v>
       </c>
-      <c r="AV2" s="171"/>
-      <c r="AW2" s="188"/>
-      <c r="AX2" s="176"/>
+      <c r="AV2" s="172"/>
+      <c r="AW2" s="187"/>
+      <c r="AX2" s="196"/>
       <c r="AY2" s="106"/>
-      <c r="AZ2" s="181" t="s">
+      <c r="AZ2" s="201" t="s">
         <v>88</v>
       </c>
-      <c r="BA2" s="183" t="s">
+      <c r="BA2" s="203" t="s">
         <v>102</v>
       </c>
-      <c r="BB2" s="183" t="s">
+      <c r="BB2" s="203" t="s">
         <v>36</v>
       </c>
-      <c r="BC2" s="185" t="s">
+      <c r="BC2" s="205" t="s">
         <v>61</v>
       </c>
-      <c r="BD2" s="166"/>
-      <c r="BE2" s="165" t="s">
+      <c r="BD2" s="190"/>
+      <c r="BE2" s="189" t="s">
         <v>88</v>
       </c>
-      <c r="BF2" s="165" t="s">
+      <c r="BF2" s="189" t="s">
         <v>102</v>
       </c>
-      <c r="BG2" s="165" t="s">
+      <c r="BG2" s="189" t="s">
         <v>36</v>
       </c>
-      <c r="BH2" s="165" t="s">
+      <c r="BH2" s="189" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:60" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="194"/>
-      <c r="B3" s="195"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="200"/>
+      <c r="A3" s="179"/>
+      <c r="B3" s="180"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="185"/>
       <c r="E3" s="50" t="s">
         <v>26</v>
       </c>
@@ -13589,18 +13578,18 @@
       <c r="AV3" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="AW3" s="189"/>
-      <c r="AX3" s="177"/>
+      <c r="AW3" s="188"/>
+      <c r="AX3" s="197"/>
       <c r="AY3" s="106"/>
-      <c r="AZ3" s="182"/>
-      <c r="BA3" s="184"/>
-      <c r="BB3" s="184"/>
-      <c r="BC3" s="186"/>
-      <c r="BD3" s="167"/>
-      <c r="BE3" s="166"/>
-      <c r="BF3" s="166"/>
-      <c r="BG3" s="166"/>
-      <c r="BH3" s="166"/>
+      <c r="AZ3" s="202"/>
+      <c r="BA3" s="204"/>
+      <c r="BB3" s="204"/>
+      <c r="BC3" s="206"/>
+      <c r="BD3" s="191"/>
+      <c r="BE3" s="190"/>
+      <c r="BF3" s="190"/>
+      <c r="BG3" s="190"/>
+      <c r="BH3" s="190"/>
     </row>
     <row r="4" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
@@ -13613,7 +13602,7 @@
         <v>101</v>
       </c>
       <c r="D4" s="57">
-        <f>ROUND(AX4-36,2)</f>
+        <f t="shared" ref="D4:D15" si="0">ROUND(AX4-36,2)</f>
         <v>20.83</v>
       </c>
       <c r="E4" s="155"/>
@@ -13685,11 +13674,11 @@
       <c r="AU4" s="67"/>
       <c r="AV4" s="68"/>
       <c r="AW4" s="59">
-        <f>SUMIF(E4:AU4,"&gt;30")</f>
+        <f t="shared" ref="AW4:AW21" si="1">SUMIF(E4:AU4,"&gt;30")</f>
         <v>341</v>
       </c>
       <c r="AX4" s="60">
-        <f>AW4/(AZ4+BE4)</f>
+        <f t="shared" ref="AX4:AX21" si="2">AW4/(AZ4+BE4)</f>
         <v>56.833333333333336</v>
       </c>
       <c r="AY4" s="96"/>
@@ -13707,18 +13696,18 @@
       </c>
       <c r="BD4" s="127"/>
       <c r="BE4" s="123">
-        <f>COUNTIF(AA4:AU4, "&gt;30")</f>
+        <f t="shared" ref="BE4:BE21" si="3">COUNTIF(AA4:AU4, "&gt;30")</f>
         <v>6</v>
       </c>
       <c r="BF4" s="143">
         <v>0</v>
       </c>
       <c r="BG4" s="123">
-        <f>SUMIF(AB4:AV4, "&lt;30")+BF4</f>
+        <f t="shared" ref="BG4:BG21" si="4">SUMIF(AB4:AV4, "&lt;30")+BF4</f>
         <v>119</v>
       </c>
       <c r="BH4" s="146">
-        <f>(BG4)/BE4</f>
+        <f t="shared" ref="BH4:BH16" si="5">(BG4)/BE4</f>
         <v>19.833333333333332</v>
       </c>
     </row>
@@ -13733,7 +13722,7 @@
         <v>34</v>
       </c>
       <c r="D5" s="64">
-        <f>ROUND(AX5-36,2)</f>
+        <f t="shared" si="0"/>
         <v>8.3800000000000008</v>
       </c>
       <c r="E5" s="65">
@@ -13845,43 +13834,43 @@
         <v>21</v>
       </c>
       <c r="AW5" s="59">
-        <f>SUMIF(E5:AU5,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>710</v>
       </c>
       <c r="AX5" s="60">
-        <f>AW5/(AZ5+BE5)</f>
+        <f t="shared" si="2"/>
         <v>44.375</v>
       </c>
       <c r="AY5" s="96"/>
       <c r="AZ5" s="69">
-        <f>COUNTIF(E5:Y5,"&gt;30")</f>
+        <f t="shared" ref="AZ5:AZ15" si="6">COUNTIF(E5:Y5,"&gt;30")</f>
         <v>7</v>
       </c>
       <c r="BA5" s="98">
         <v>2</v>
       </c>
       <c r="BB5" s="99">
-        <f>SUMIF(E5:Z5,"&lt;30")+BA5</f>
+        <f t="shared" ref="BB5:BB15" si="7">SUMIF(E5:Z5,"&lt;30")+BA5</f>
         <v>126</v>
       </c>
       <c r="BC5" s="108">
-        <f>(BB5)/AZ5</f>
+        <f t="shared" ref="BC5:BC15" si="8">(BB5)/AZ5</f>
         <v>18</v>
       </c>
       <c r="BD5" s="127"/>
       <c r="BE5" s="132">
-        <f>COUNTIF(AA5:AU5, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="BF5" s="144">
         <v>2</v>
       </c>
       <c r="BG5" s="132">
-        <f>SUMIF(AB5:AV5, "&lt;30")+BF5</f>
+        <f t="shared" si="4"/>
         <v>176</v>
       </c>
       <c r="BH5" s="147">
-        <f>(BG5)/BE5</f>
+        <f t="shared" si="5"/>
         <v>19.555555555555557</v>
       </c>
     </row>
@@ -13896,7 +13885,7 @@
         <v>34</v>
       </c>
       <c r="D6" s="64">
-        <f>ROUND(AX6-36,2)</f>
+        <f t="shared" si="0"/>
         <v>12.59</v>
       </c>
       <c r="E6" s="75">
@@ -14012,45 +14001,45 @@
         <v>18</v>
       </c>
       <c r="AW6" s="59">
-        <f>SUMIF(E6:AU6,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>826</v>
       </c>
       <c r="AX6" s="60">
-        <f>AW6/(AZ6+BE6)</f>
+        <f t="shared" si="2"/>
         <v>48.588235294117645</v>
       </c>
       <c r="AY6" s="96"/>
       <c r="AZ6" s="69">
-        <f>COUNTIF(E6:Y6,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="BA6" s="98">
         <v>2</v>
       </c>
       <c r="BB6" s="99">
-        <f>SUMIF(E6:Z6,"&lt;30")+BA6</f>
+        <f t="shared" si="7"/>
         <v>206</v>
       </c>
       <c r="BC6" s="108">
-        <f>(BB6)/AZ6</f>
+        <f t="shared" si="8"/>
         <v>18.727272727272727</v>
       </c>
       <c r="BD6" s="129" t="s">
         <v>108</v>
       </c>
       <c r="BE6" s="132">
-        <f>COUNTIF(AA6:AU6, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="BF6" s="144">
         <v>3</v>
       </c>
       <c r="BG6" s="132">
-        <f>SUMIF(AB6:AV6, "&lt;30")+BF6</f>
+        <f t="shared" si="4"/>
         <v>117</v>
       </c>
       <c r="BH6" s="147">
-        <f>(BG6)/BE6</f>
+        <f t="shared" si="5"/>
         <v>19.5</v>
       </c>
     </row>
@@ -14065,7 +14054,7 @@
         <v>34</v>
       </c>
       <c r="D7" s="64">
-        <f>ROUND(AX7-36,2)</f>
+        <f t="shared" si="0"/>
         <v>14.87</v>
       </c>
       <c r="E7" s="65">
@@ -14173,43 +14162,43 @@
         <v>11</v>
       </c>
       <c r="AW7" s="59">
-        <f>SUMIF(E7:AU7,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>763</v>
       </c>
       <c r="AX7" s="60">
-        <f>AW7/(AZ7+BE7)</f>
+        <f t="shared" si="2"/>
         <v>50.866666666666667</v>
       </c>
       <c r="AY7" s="96"/>
       <c r="AZ7" s="69">
-        <f>COUNTIF(E7:Y7,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="BA7" s="98">
         <v>0</v>
       </c>
       <c r="BB7" s="99">
-        <f>SUMIF(E7:Z7,"&lt;30")+BA7</f>
+        <f t="shared" si="7"/>
         <v>166</v>
       </c>
       <c r="BC7" s="108">
-        <f>(BB7)/AZ7</f>
+        <f t="shared" si="8"/>
         <v>18.444444444444443</v>
       </c>
       <c r="BD7" s="127"/>
       <c r="BE7" s="132">
-        <f>COUNTIF(AA7:AU7, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="BF7" s="144">
         <v>0</v>
       </c>
       <c r="BG7" s="132">
-        <f>SUMIF(AB7:AV7, "&lt;30")+BF7</f>
+        <f t="shared" si="4"/>
         <v>116</v>
       </c>
       <c r="BH7" s="147">
-        <f>(BG7)/BE7</f>
+        <f t="shared" si="5"/>
         <v>19.333333333333332</v>
       </c>
     </row>
@@ -14224,7 +14213,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="64">
-        <f>ROUND(AX8-36,2)</f>
+        <f t="shared" si="0"/>
         <v>1.93</v>
       </c>
       <c r="E8" s="65">
@@ -14325,50 +14314,50 @@
       </c>
       <c r="AS8" s="159"/>
       <c r="AT8" s="68"/>
-      <c r="AU8" s="161">
+      <c r="AU8" s="158">
         <v>41</v>
       </c>
       <c r="AV8" s="66">
         <v>15</v>
       </c>
       <c r="AW8" s="59">
-        <f>SUMIF(E8:AU8,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>569</v>
       </c>
       <c r="AX8" s="60">
-        <f>AW8/(AZ8+BE8)</f>
+        <f t="shared" si="2"/>
         <v>37.93333333333333</v>
       </c>
       <c r="AY8" s="96"/>
       <c r="AZ8" s="69">
-        <f>COUNTIF(E8:Y8,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="BA8" s="98">
         <v>5</v>
       </c>
       <c r="BB8" s="99">
-        <f>SUMIF(E8:Z8,"&lt;30")+BA8</f>
+        <f t="shared" si="7"/>
         <v>127</v>
       </c>
       <c r="BC8" s="108">
-        <f>(BB8)/AZ8</f>
+        <f t="shared" si="8"/>
         <v>18.142857142857142</v>
       </c>
       <c r="BD8" s="128"/>
-      <c r="BE8" s="210">
-        <f>COUNTIF(AA8:AU8, "&gt;30")</f>
+      <c r="BE8" s="164">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="BF8" s="144">
         <v>9</v>
       </c>
       <c r="BG8" s="132">
-        <f>SUMIF(AB8:AV8, "&lt;30")+BF8</f>
+        <f t="shared" si="4"/>
         <v>154</v>
       </c>
       <c r="BH8" s="147">
-        <f>(BG8)/BE8</f>
+        <f t="shared" si="5"/>
         <v>19.25</v>
       </c>
     </row>
@@ -14383,7 +14372,7 @@
         <v>34</v>
       </c>
       <c r="D9" s="64">
-        <f>ROUND(AX9-36,2)</f>
+        <f t="shared" si="0"/>
         <v>10.62</v>
       </c>
       <c r="E9" s="67"/>
@@ -14483,45 +14472,45 @@
         <v>20</v>
       </c>
       <c r="AW9" s="59">
-        <f>SUMIF(E9:AU9,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>606</v>
       </c>
       <c r="AX9" s="60">
-        <f>AW9/(AZ9+BE9)</f>
+        <f t="shared" si="2"/>
         <v>46.615384615384613</v>
       </c>
       <c r="AY9" s="96"/>
       <c r="AZ9" s="69">
-        <f>COUNTIF(E9:Y9,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="BA9" s="98">
         <v>2</v>
       </c>
       <c r="BB9" s="99">
-        <f>SUMIF(E9:Z9,"&lt;30")+BA9</f>
+        <f t="shared" si="7"/>
         <v>115</v>
       </c>
       <c r="BC9" s="108">
-        <f>(BB9)/AZ9</f>
+        <f t="shared" si="8"/>
         <v>19.166666666666668</v>
       </c>
       <c r="BD9" s="129" t="s">
         <v>106</v>
       </c>
       <c r="BE9" s="132">
-        <f>COUNTIF(AA9:AU9, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="BF9" s="144">
         <v>1</v>
       </c>
       <c r="BG9" s="132">
-        <f>SUMIF(AB9:AV9, "&lt;30")+BF9</f>
+        <f t="shared" si="4"/>
         <v>127</v>
       </c>
       <c r="BH9" s="147">
-        <f>(BG9)/BE9</f>
+        <f t="shared" si="5"/>
         <v>18.142857142857142</v>
       </c>
     </row>
@@ -14536,7 +14525,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="64">
-        <f>ROUND(AX10-36,2)</f>
+        <f t="shared" si="0"/>
         <v>12.64</v>
       </c>
       <c r="E10" s="65">
@@ -14640,43 +14629,43 @@
         <v>14</v>
       </c>
       <c r="AW10" s="59">
-        <f>SUMIF(E10:AU10,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>681</v>
       </c>
       <c r="AX10" s="60">
-        <f>AW10/(AZ10+BE10)</f>
+        <f t="shared" si="2"/>
         <v>48.642857142857146</v>
       </c>
       <c r="AY10" s="96"/>
       <c r="AZ10" s="69">
-        <f>COUNTIF(E10:Y10,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="BA10" s="98">
         <v>2</v>
       </c>
       <c r="BB10" s="99">
-        <f>SUMIF(E10:Z10,"&lt;30")+BA10</f>
+        <f t="shared" si="7"/>
         <v>127</v>
       </c>
       <c r="BC10" s="108">
-        <f>(BB10)/AZ10</f>
+        <f t="shared" si="8"/>
         <v>18.142857142857142</v>
       </c>
       <c r="BD10" s="128"/>
-      <c r="BE10" s="209">
-        <f>COUNTIF(AA10:AU10, "&gt;30")</f>
+      <c r="BE10" s="163">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="BF10" s="144">
         <v>1</v>
       </c>
       <c r="BG10" s="132">
-        <f>SUMIF(AB10:AV10, "&lt;30")+BF10</f>
+        <f t="shared" si="4"/>
         <v>127</v>
       </c>
       <c r="BH10" s="147">
-        <f>(BG10)/BE10</f>
+        <f t="shared" si="5"/>
         <v>18.142857142857142</v>
       </c>
     </row>
@@ -14691,7 +14680,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="64">
-        <f>ROUND(AX11-36,2)</f>
+        <f t="shared" si="0"/>
         <v>14.72</v>
       </c>
       <c r="E11" s="65">
@@ -14811,45 +14800,45 @@
       <c r="AU11" s="67"/>
       <c r="AV11" s="68"/>
       <c r="AW11" s="59">
-        <f>SUMIF(E11:AU11,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>913</v>
       </c>
       <c r="AX11" s="60">
-        <f>AW11/(AZ11+BE11)</f>
+        <f t="shared" si="2"/>
         <v>50.722222222222221</v>
       </c>
       <c r="AY11" s="96"/>
       <c r="AZ11" s="69">
-        <f>COUNTIF(E11:Y11,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="BA11" s="98">
         <v>1</v>
       </c>
       <c r="BB11" s="99">
-        <f>SUMIF(E11:Z11,"&lt;30")+BA11</f>
+        <f t="shared" si="7"/>
         <v>189</v>
       </c>
       <c r="BC11" s="108">
-        <f>(BB11)/AZ11</f>
+        <f t="shared" si="8"/>
         <v>18.899999999999999</v>
       </c>
       <c r="BD11" s="129" t="s">
         <v>107</v>
       </c>
       <c r="BE11" s="132">
-        <f>COUNTIF(AA11:AU11, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="BF11" s="144">
         <v>0</v>
       </c>
       <c r="BG11" s="132">
-        <f>SUMIF(AB11:AV11, "&lt;30")+BF11</f>
+        <f t="shared" si="4"/>
         <v>139</v>
       </c>
       <c r="BH11" s="147">
-        <f>(BG11)/BE11</f>
+        <f t="shared" si="5"/>
         <v>17.375</v>
       </c>
     </row>
@@ -14864,7 +14853,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="64">
-        <f>ROUND(AX12-36,2)</f>
+        <f t="shared" si="0"/>
         <v>21.75</v>
       </c>
       <c r="E12" s="65">
@@ -14976,43 +14965,43 @@
       <c r="AU12" s="67"/>
       <c r="AV12" s="68"/>
       <c r="AW12" s="59">
-        <f>SUMIF(E12:AU12,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>924</v>
       </c>
       <c r="AX12" s="60">
-        <f>AW12/(AZ12+BE12)</f>
+        <f t="shared" si="2"/>
         <v>57.75</v>
       </c>
       <c r="AY12" s="96"/>
       <c r="AZ12" s="69">
-        <f>COUNTIF(E12:Y12,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="BA12" s="98">
         <v>0</v>
       </c>
       <c r="BB12" s="99">
-        <f>SUMIF(E12:Z12,"&lt;30")+BA12</f>
+        <f t="shared" si="7"/>
         <v>166</v>
       </c>
       <c r="BC12" s="108">
-        <f>(BB12)/AZ12</f>
+        <f t="shared" si="8"/>
         <v>18.444444444444443</v>
       </c>
       <c r="BD12" s="128"/>
       <c r="BE12" s="132">
-        <f>COUNTIF(AA12:AU12, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="BF12" s="144">
         <v>0</v>
       </c>
       <c r="BG12" s="132">
-        <f>SUMIF(AB12:AV12, "&lt;30")+BF12</f>
+        <f t="shared" si="4"/>
         <v>114</v>
       </c>
       <c r="BH12" s="147">
-        <f>(BG12)/BE12</f>
+        <f t="shared" si="5"/>
         <v>16.285714285714285</v>
       </c>
     </row>
@@ -15027,7 +15016,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="64">
-        <f>ROUND(AX13-36,2)</f>
+        <f t="shared" si="0"/>
         <v>14.9</v>
       </c>
       <c r="E13" s="67"/>
@@ -15115,43 +15104,43 @@
         <v>19</v>
       </c>
       <c r="AW13" s="59">
-        <f>SUMIF(E13:AU13,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>509</v>
       </c>
       <c r="AX13" s="60">
-        <f>AW13/(AZ13+BE13)</f>
+        <f t="shared" si="2"/>
         <v>50.9</v>
       </c>
       <c r="AY13" s="96"/>
       <c r="AZ13" s="69">
-        <f>COUNTIF(E13:Y13,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="BA13" s="98">
         <v>0</v>
       </c>
       <c r="BB13" s="99">
-        <f>SUMIF(E13:Z13,"&lt;30")+BA13</f>
+        <f t="shared" si="7"/>
         <v>88</v>
       </c>
       <c r="BC13" s="108">
-        <f>(BB13)/AZ13</f>
+        <f t="shared" si="8"/>
         <v>17.600000000000001</v>
       </c>
       <c r="BD13" s="128"/>
-      <c r="BE13" s="211">
-        <f>COUNTIF(AA13:AU13, "&gt;30")</f>
+      <c r="BE13" s="165">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BF13" s="144">
         <v>0</v>
       </c>
       <c r="BG13" s="132">
-        <f>SUMIF(AB13:AV13, "&lt;30")+BF13</f>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
       <c r="BH13" s="147">
-        <f>(BG13)/BE13</f>
+        <f t="shared" si="5"/>
         <v>18.600000000000001</v>
       </c>
     </row>
@@ -15166,7 +15155,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="64">
-        <f>ROUND(AX14-36,2)</f>
+        <f t="shared" si="0"/>
         <v>21.5</v>
       </c>
       <c r="E14" s="65">
@@ -15258,43 +15247,43 @@
       <c r="AU14" s="67"/>
       <c r="AV14" s="68"/>
       <c r="AW14" s="59">
-        <f>SUMIF(E14:AU14,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>575</v>
       </c>
       <c r="AX14" s="60">
-        <f>AW14/(AZ14+BE14)</f>
+        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="AY14" s="96"/>
       <c r="AZ14" s="69">
-        <f>COUNTIF(E14:Y14,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="BA14" s="98">
         <v>1</v>
       </c>
       <c r="BB14" s="99">
-        <f>SUMIF(E14:Z14,"&lt;30")+BA14</f>
+        <f t="shared" si="7"/>
         <v>102</v>
       </c>
       <c r="BC14" s="108">
-        <f>(BB14)/AZ14</f>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="BD14" s="128"/>
-      <c r="BE14" s="211">
-        <f>COUNTIF(AA14:AU14, "&gt;30")</f>
+      <c r="BE14" s="165">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="BF14" s="144">
         <v>0</v>
       </c>
       <c r="BG14" s="132">
-        <f>SUMIF(AB14:AV14, "&lt;30")+BF14</f>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="BH14" s="147">
-        <f>(BG14)/BE14</f>
+        <f t="shared" si="5"/>
         <v>17.75</v>
       </c>
     </row>
@@ -15309,7 +15298,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="64">
-        <f>ROUND(AX15-36,2)</f>
+        <f t="shared" si="0"/>
         <v>16.920000000000002</v>
       </c>
       <c r="E15" s="65">
@@ -15409,43 +15398,43 @@
         <v>15</v>
       </c>
       <c r="AW15" s="59">
-        <f>SUMIF(E15:AU15,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>688</v>
       </c>
       <c r="AX15" s="60">
-        <f>AW15/(AZ15+BE15)</f>
+        <f t="shared" si="2"/>
         <v>52.92307692307692</v>
       </c>
       <c r="AY15" s="96"/>
       <c r="AZ15" s="69">
-        <f>COUNTIF(E15:Y15,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="BA15" s="98">
         <v>0</v>
       </c>
       <c r="BB15" s="99">
-        <f>SUMIF(E15:Z15,"&lt;30")+BA15</f>
+        <f t="shared" si="7"/>
         <v>146</v>
       </c>
       <c r="BC15" s="108">
-        <f>(BB15)/AZ15</f>
+        <f t="shared" si="8"/>
         <v>18.25</v>
       </c>
       <c r="BD15" s="128"/>
-      <c r="BE15" s="211">
-        <f>COUNTIF(AA15:AU15, "&gt;30")</f>
+      <c r="BE15" s="165">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BF15" s="144">
         <v>1</v>
       </c>
       <c r="BG15" s="132">
-        <f>SUMIF(AB15:AV15, "&lt;30")+BF15</f>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="BH15" s="147">
-        <f>(BG15)/BE15</f>
+        <f t="shared" si="5"/>
         <v>16.2</v>
       </c>
     </row>
@@ -15509,11 +15498,11 @@
       <c r="AU16" s="67"/>
       <c r="AV16" s="68"/>
       <c r="AW16" s="59">
-        <f>SUMIF(E16:AU16,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="AX16" s="60">
-        <f>AW16/(AZ16+BE16)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="AY16" s="96"/>
@@ -15522,19 +15511,19 @@
       <c r="BB16" s="99"/>
       <c r="BC16" s="108"/>
       <c r="BD16" s="128"/>
-      <c r="BE16" s="211">
-        <f>COUNTIF(AA16:AU16, "&gt;30")</f>
+      <c r="BE16" s="165">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="BF16" s="144">
         <v>0</v>
       </c>
       <c r="BG16" s="132">
-        <f>SUMIF(AB16:AV16, "&lt;30")+BF16</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BH16" s="147">
-        <f>(BG16)/BE16</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -15639,11 +15628,11 @@
       <c r="AU17" s="67"/>
       <c r="AV17" s="68"/>
       <c r="AW17" s="59">
-        <f>SUMIF(E17:AU17,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>399</v>
       </c>
       <c r="AX17" s="60">
-        <f>AW17/(AZ17+BE17)</f>
+        <f t="shared" si="2"/>
         <v>44.333333333333336</v>
       </c>
       <c r="AY17" s="96"/>
@@ -15663,15 +15652,15 @@
         <v>18.777777777777779</v>
       </c>
       <c r="BD17" s="130"/>
-      <c r="BE17" s="211">
-        <f>COUNTIF(AA17:AU17, "&gt;30")</f>
+      <c r="BE17" s="165">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BF17" s="144">
         <v>0</v>
       </c>
       <c r="BG17" s="132">
-        <f>SUMIF(AB17:AV17, "&lt;30")+BF17</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BH17" s="147">
@@ -15740,11 +15729,11 @@
       <c r="AU18" s="67"/>
       <c r="AV18" s="68"/>
       <c r="AW18" s="59">
-        <f>SUMIF(E18:AU18,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="AX18" s="60">
-        <f>AW18/(AZ18+BE18)</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="AY18" s="96"/>
@@ -15764,15 +15753,15 @@
         <v>0</v>
       </c>
       <c r="BD18" s="128"/>
-      <c r="BE18" s="211">
-        <f>COUNTIF(AA18:AU18, "&gt;30")</f>
+      <c r="BE18" s="165">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BF18" s="144">
         <v>0</v>
       </c>
       <c r="BG18" s="132">
-        <f>SUMIF(AB18:AV18, "&lt;30")+BF18</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BH18" s="147">
@@ -15841,11 +15830,11 @@
       <c r="AU19" s="67"/>
       <c r="AV19" s="68"/>
       <c r="AW19" s="59">
-        <f>SUMIF(E19:AU19,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="AX19" s="60">
-        <f>AW19/(AZ19+BE19)</f>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="AY19" s="96"/>
@@ -15865,15 +15854,15 @@
         <v>0</v>
       </c>
       <c r="BD19" s="128"/>
-      <c r="BE19" s="211">
-        <f>COUNTIF(AA19:AU19, "&gt;30")</f>
+      <c r="BE19" s="165">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BF19" s="132">
         <v>0</v>
       </c>
       <c r="BG19" s="132">
-        <f>SUMIF(AB19:AV19, "&lt;30")+BF19</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BH19" s="147">
@@ -15955,11 +15944,11 @@
       <c r="AU20" s="67"/>
       <c r="AV20" s="68"/>
       <c r="AW20" s="59">
-        <f>SUMIF(E20:AU20,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>217</v>
       </c>
       <c r="AX20" s="60">
-        <f>AW20/(AZ20+BE20)</f>
+        <f t="shared" si="2"/>
         <v>54.25</v>
       </c>
       <c r="AY20" s="96"/>
@@ -15979,15 +15968,15 @@
         <v>18</v>
       </c>
       <c r="BD20" s="128"/>
-      <c r="BE20" s="211">
-        <f>COUNTIF(AA20:AU20, "&gt;30")</f>
+      <c r="BE20" s="165">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BF20" s="144">
         <v>0</v>
       </c>
       <c r="BG20" s="132">
-        <f>SUMIF(AB20:AV20, "&lt;30")+BF20</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BH20" s="147">
@@ -16060,11 +16049,11 @@
       <c r="AU21" s="67"/>
       <c r="AV21" s="68"/>
       <c r="AW21" s="59">
-        <f>SUMIF(E21:AU21,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>123</v>
       </c>
       <c r="AX21" s="60">
-        <f>AW21/(AZ21+BE21)</f>
+        <f t="shared" si="2"/>
         <v>61.5</v>
       </c>
       <c r="AY21" s="96"/>
@@ -16084,15 +16073,15 @@
         <v>0</v>
       </c>
       <c r="BD21" s="131"/>
-      <c r="BE21" s="211">
-        <f>COUNTIF(AA21:AU21, "&gt;30")</f>
+      <c r="BE21" s="165">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="BF21" s="145">
         <v>0</v>
       </c>
       <c r="BG21" s="133">
-        <f>SUMIF(AB21:AV21, "&lt;30")+BF21</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BH21" s="148">
@@ -16290,12 +16279,12 @@
       <c r="AS25" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="AU25" s="207"/>
-      <c r="AV25" s="208" t="s">
+      <c r="AU25" s="161"/>
+      <c r="AV25" s="162" t="s">
         <v>126</v>
       </c>
-      <c r="AW25" s="208"/>
-      <c r="AX25" s="208"/>
+      <c r="AW25" s="162"/>
+      <c r="AX25" s="162"/>
     </row>
     <row r="26" spans="1:60" x14ac:dyDescent="0.25">
       <c r="D26" s="92" t="s">
@@ -16335,11 +16324,55 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:BH21">
-    <sortCondition descending="1" sortBy="cellColor" ref="BE4:BE21" dxfId="1"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="BE4:BE21" dxfId="0"/>
     <sortCondition descending="1" ref="BH4:BH21"/>
     <sortCondition ref="AX4:AX21"/>
   </sortState>
   <mergeCells count="60">
+    <mergeCell ref="BD1:BD3"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="BE1:BH1"/>
+    <mergeCell ref="BE2:BE3"/>
+    <mergeCell ref="BF2:BF3"/>
+    <mergeCell ref="BG2:BG3"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="AX1:AX3"/>
+    <mergeCell ref="AZ1:BC1"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AW1:AW3"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="E2:F2"/>
@@ -16356,54 +16389,13 @@
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AW1:AW3"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AS1:AT1"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AU1:AV1"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="BD1:BD3"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="BE1:BH1"/>
-    <mergeCell ref="BE2:BE3"/>
-    <mergeCell ref="BF2:BF3"/>
-    <mergeCell ref="BG2:BG3"/>
-    <mergeCell ref="BH2:BH3"/>
-    <mergeCell ref="AX1:AX3"/>
-    <mergeCell ref="AZ1:BC1"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="BC2:BC3"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AQ2:AR2"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="BE5:BE13 BE15 BE17" formulaRange="1"/>
+  </ignoredErrors>
   <webPublishItems count="1">
     <webPublishItem id="24146" divId="Bottoms Up 2024 League Stats - Week 11_24146" sourceType="sheet" destinationFile="C:\DATA\CODE\golf-league-site\public\results\Bottoms Up 2024 League Stats - Week 11.htm" title="WEEK 11" autoRepublish="1"/>
   </webPublishItems>
@@ -16437,23 +16429,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -16467,23 +16459,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -17807,23 +17799,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -17837,23 +17829,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -19130,23 +19122,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -19160,23 +19152,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -20453,23 +20445,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -20483,23 +20475,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -21765,23 +21757,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -21795,23 +21787,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -22804,23 +22796,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -22834,23 +22826,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -25067,23 +25059,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -25097,23 +25089,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -26639,23 +26631,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -26669,23 +26661,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -28300,23 +28292,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -28330,23 +28322,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -29752,23 +29744,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -29782,23 +29774,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -31147,23 +31139,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -31177,23 +31169,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -31950,9 +31942,9 @@
       </c>
       <c r="O15" s="15"/>
       <c r="P15" s="36"/>
-      <c r="Q15" s="203"/>
-      <c r="R15" s="204"/>
-      <c r="S15" s="205"/>
+      <c r="Q15" s="207"/>
+      <c r="R15" s="208"/>
+      <c r="S15" s="209"/>
       <c r="T15" s="41">
         <v>35</v>
       </c>
@@ -32796,23 +32788,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="166" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="163"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -32826,23 +32818,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>

</xml_diff>